<commit_message>
committing on 21apr - common Library with nested arraylist comparison, neo4j code cleanup, ExtraFunctions keyword to dump extra functions
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/readUIResultsData.xlsx
+++ b/CTDC_Automation/TestData/readUIResultsData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Katalon_POC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F00FB5-8D4C-4187-A441-DA561940AE64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86316F77-606E-449E-AF89-9E49DC649926}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="1940" windowWidth="14400" windowHeight="7400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="exceltrial2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="119">
   <si>
     <t>Case ID</t>
   </si>
@@ -340,6 +340,48 @@
   </si>
   <si>
     <t>CTDC-46500</t>
+  </si>
+  <si>
+    <t>CTDC-46654</t>
+  </si>
+  <si>
+    <t>CTDC-46681</t>
+  </si>
+  <si>
+    <t>CTDC-46730</t>
+  </si>
+  <si>
+    <t>Adenocarcinoma of the cervix</t>
+  </si>
+  <si>
+    <t>CTDC-46749</t>
+  </si>
+  <si>
+    <t>CTDC-46779</t>
+  </si>
+  <si>
+    <t>CTDC-46828</t>
+  </si>
+  <si>
+    <t>Female reproductive system cancer, NOS</t>
+  </si>
+  <si>
+    <t>AMERICAN_INDIAN_OR_ALASKA_NATIVE</t>
+  </si>
+  <si>
+    <t>CTDC-46968</t>
+  </si>
+  <si>
+    <t>CTDC-47398</t>
+  </si>
+  <si>
+    <t>Hurthle cell neoplasm (thyroid)</t>
+  </si>
+  <si>
+    <t>CTDC-47810</t>
+  </si>
+  <si>
+    <t>CTDC-47986</t>
   </si>
 </sst>
 </file>
@@ -656,54 +698,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E7D7C2-E254-4733-92E5-C9C86D34788A}">
-  <dimension ref="A1:H61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6A8672-6039-4A41-803B-B513C91F44C7}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -715,21 +758,21 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -741,7 +784,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -750,27 +793,27 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -781,19 +824,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -807,33 +850,33 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -845,7 +888,7 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
         <v>18</v>
@@ -854,12 +897,12 @@
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -871,7 +914,7 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -880,12 +923,12 @@
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -897,36 +940,36 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -937,77 +980,77 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
         <v>23</v>
@@ -1015,19 +1058,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
@@ -1041,22 +1084,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1067,7 +1110,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -1079,7 +1122,7 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
@@ -1093,25 +1136,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H17" t="s">
         <v>23</v>
@@ -1119,7 +1162,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -1131,7 +1174,7 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="F18" t="s">
         <v>18</v>
@@ -1145,71 +1188,71 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G20" t="s">
         <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
         <v>18</v>
@@ -1218,12 +1261,12 @@
         <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -1238,7 +1281,7 @@
         <v>32</v>
       </c>
       <c r="F22" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
@@ -1249,19 +1292,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F23" t="s">
         <v>18</v>
@@ -1275,7 +1318,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -1287,21 +1330,21 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s">
         <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -1313,13 +1356,13 @@
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H25" t="s">
         <v>23</v>
@@ -1327,25 +1370,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H26" t="s">
         <v>23</v>
@@ -1353,7 +1396,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
@@ -1365,36 +1408,36 @@
         <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G28" t="s">
         <v>14</v>
@@ -1405,7 +1448,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
@@ -1417,7 +1460,7 @@
         <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F29" t="s">
         <v>18</v>
@@ -1431,22 +1474,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G30" t="s">
         <v>37</v>
@@ -1457,7 +1500,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
@@ -1469,10 +1512,10 @@
         <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="F31" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
         <v>14</v>
@@ -1483,19 +1526,19 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="F32" t="s">
         <v>18</v>
@@ -1509,48 +1552,48 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="F33" t="s">
         <v>18</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H33" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="F34" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G34" t="s">
         <v>14</v>
@@ -1561,25 +1604,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="F35" t="s">
         <v>18</v>
       </c>
       <c r="G35" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="H35" t="s">
         <v>23</v>
@@ -1587,22 +1630,22 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="F36" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G36" t="s">
         <v>14</v>
@@ -1613,7 +1656,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
@@ -1639,7 +1682,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
@@ -1651,7 +1694,7 @@
         <v>21</v>
       </c>
       <c r="E38" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="F38" t="s">
         <v>18</v>
@@ -1665,7 +1708,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
@@ -1677,10 +1720,10 @@
         <v>21</v>
       </c>
       <c r="E39" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="F39" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
@@ -1691,19 +1734,19 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E40" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F40" t="s">
         <v>18</v>
@@ -1717,22 +1760,22 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E41" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="F41" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G41" t="s">
         <v>14</v>
@@ -1743,19 +1786,19 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E42" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="F42" t="s">
         <v>18</v>
@@ -1769,25 +1812,25 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E43" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F43" t="s">
         <v>18</v>
       </c>
       <c r="G43" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="H43" t="s">
         <v>23</v>
@@ -1795,7 +1838,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
@@ -1807,13 +1850,13 @@
         <v>21</v>
       </c>
       <c r="E44" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="F44" t="s">
         <v>18</v>
       </c>
       <c r="G44" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="H44" t="s">
         <v>23</v>
@@ -1821,25 +1864,25 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="F45" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G45" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H45" t="s">
         <v>23</v>
@@ -1847,7 +1890,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
@@ -1859,13 +1902,13 @@
         <v>21</v>
       </c>
       <c r="E46" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="F46" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G46" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H46" t="s">
         <v>23</v>
@@ -1873,33 +1916,33 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E47" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="F47" t="s">
         <v>18</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
@@ -1911,10 +1954,10 @@
         <v>21</v>
       </c>
       <c r="E48" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="F48" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G48" t="s">
         <v>14</v>
@@ -1925,33 +1968,33 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F49" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G49" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="H49" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
@@ -1963,7 +2006,7 @@
         <v>11</v>
       </c>
       <c r="E50" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>
@@ -1972,24 +2015,24 @@
         <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F51" t="s">
         <v>13</v>
@@ -1998,12 +2041,12 @@
         <v>14</v>
       </c>
       <c r="H51" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
@@ -2015,7 +2058,7 @@
         <v>21</v>
       </c>
       <c r="E52" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="F52" t="s">
         <v>18</v>
@@ -2029,19 +2072,19 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E53" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="F53" t="s">
         <v>18</v>
@@ -2055,7 +2098,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
@@ -2067,13 +2110,13 @@
         <v>21</v>
       </c>
       <c r="E54" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="F54" t="s">
         <v>18</v>
       </c>
       <c r="G54" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="H54" t="s">
         <v>23</v>
@@ -2081,7 +2124,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
         <v>9</v>
@@ -2093,7 +2136,7 @@
         <v>21</v>
       </c>
       <c r="E55" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="F55" t="s">
         <v>18</v>
@@ -2107,19 +2150,19 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E56" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F56" t="s">
         <v>13</v>
@@ -2133,7 +2176,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
@@ -2145,13 +2188,13 @@
         <v>11</v>
       </c>
       <c r="E57" t="s">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="F57" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="H57" t="s">
         <v>23</v>
@@ -2159,7 +2202,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
@@ -2171,13 +2214,13 @@
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F58" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H58" t="s">
         <v>23</v>
@@ -2185,7 +2228,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
@@ -2197,13 +2240,13 @@
         <v>21</v>
       </c>
       <c r="E59" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="F59" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H59" t="s">
         <v>23</v>
@@ -2211,25 +2254,25 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E60" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="F60" t="s">
         <v>18</v>
       </c>
       <c r="G60" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="H60" t="s">
         <v>23</v>
@@ -2237,31 +2280,396 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="F61" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G61" t="s">
+        <v>48</v>
+      </c>
+      <c r="H61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>100</v>
+      </c>
+      <c r="F62" t="s">
+        <v>18</v>
+      </c>
+      <c r="G62" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" t="s">
+        <v>61</v>
+      </c>
+      <c r="F63" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" t="s">
+        <v>37</v>
+      </c>
+      <c r="H66" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" t="s">
         <v>44</v>
       </c>
-      <c r="H61" t="s">
-        <v>23</v>
+      <c r="H67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" t="s">
+        <v>18</v>
+      </c>
+      <c r="G68" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>98</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" t="s">
+        <v>14</v>
+      </c>
+      <c r="H70" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" t="s">
+        <v>108</v>
+      </c>
+      <c r="F71" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" t="s">
+        <v>15</v>
+      </c>
+      <c r="H71" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H71">
+    <sortCondition descending="1" ref="E1"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="A23" r:id="rId1" location="/case/CTDC-44595" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-44595" xr:uid="{5A3E2522-7B8A-4EA9-A771-E8D5A1E32423}"/>
+    <hyperlink ref="B23" r:id="rId2" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{7F4D49F6-510E-4AA2-81E9-2EB9F9D3BD0F}"/>
+    <hyperlink ref="A40" r:id="rId3" location="/case/CTDC-44638" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-44638" xr:uid="{8DB07991-2A29-499C-8407-6938409EB037}"/>
+    <hyperlink ref="B40" r:id="rId4" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{3AD67851-B045-4D8F-AA37-295E655303B5}"/>
+    <hyperlink ref="A8" r:id="rId5" location="/case/CTDC-44641" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-44641" xr:uid="{0B01772E-6605-420D-808B-E5A15CE3B650}"/>
+    <hyperlink ref="B8" r:id="rId6" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{D397AE03-F746-4D4A-8337-30732C6F396C}"/>
+    <hyperlink ref="A9" r:id="rId7" location="/case/CTDC-44670" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-44670" xr:uid="{53BD1A07-DF58-43F4-9710-C534AD4430F7}"/>
+    <hyperlink ref="B9" r:id="rId8" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{F2C5C4D1-6AB7-42F7-9732-04EEEBD2D7C5}"/>
+    <hyperlink ref="A57" r:id="rId9" location="/case/CTDC-44695" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-44695" xr:uid="{921A7DA2-8F50-4D99-B643-93101200AD54}"/>
+    <hyperlink ref="B57" r:id="rId10" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{B72F031D-C240-4382-8BB5-C618272760A2}"/>
+    <hyperlink ref="A63" r:id="rId11" location="/case/CTDC-44767" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-44767" xr:uid="{6B801343-4D71-4362-B7E5-06CA9CE228DA}"/>
+    <hyperlink ref="B63" r:id="rId12" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{630CD89A-0E7E-48DB-BF0C-046858E6AD38}"/>
+    <hyperlink ref="A4" r:id="rId13" location="/case/CTDC-44792" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-44792" xr:uid="{24D60DBF-64F2-47E7-9209-F796EDB187CE}"/>
+    <hyperlink ref="B4" r:id="rId14" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{6C6210B3-3D13-4DF0-BCAD-9EC45FCC728A}"/>
+    <hyperlink ref="A53" r:id="rId15" location="/case/CTDC-44825" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-44825" xr:uid="{7BEE9C20-515E-442D-B4B0-09270A5E7858}"/>
+    <hyperlink ref="B53" r:id="rId16" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{474C379B-E94C-467D-95B6-FA1F0482036A}"/>
+    <hyperlink ref="A25" r:id="rId17" location="/case/CTDC-44895" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-44895" xr:uid="{0A8E634E-58C7-4E76-ABF8-F1A7768E3031}"/>
+    <hyperlink ref="B25" r:id="rId18" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{6D2B3D77-E1C3-41A5-B5B1-6FD71D7A32FB}"/>
+    <hyperlink ref="A18" r:id="rId19" location="/case/CTDC-44976" display="/case/CTDC-44976" xr:uid="{DD2162C1-0D37-4C57-AE39-EA8C73DDF91D}"/>
+    <hyperlink ref="B18" r:id="rId20" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{BB08F83A-4335-41C9-AAA4-41027F7B1198}"/>
+    <hyperlink ref="A52" r:id="rId21" location="/case/CTDC-45101" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45101" xr:uid="{26383887-C673-4D46-8E4A-76162BBD700C}"/>
+    <hyperlink ref="B52" r:id="rId22" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{8AC0B13E-3B50-4B3D-84C4-972E1E718BF3}"/>
+    <hyperlink ref="A41" r:id="rId23" location="/case/CTDC-45175" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45175" xr:uid="{9BE2F198-CEA4-4117-A760-888D5E1BB294}"/>
+    <hyperlink ref="B41" r:id="rId24" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{BDBE689F-71CB-4ED7-9115-EF28119DCFA3}"/>
+    <hyperlink ref="A10" r:id="rId25" location="/case/CTDC-45209" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45209" xr:uid="{4727A5F0-4316-4B54-9462-91913524B59B}"/>
+    <hyperlink ref="B10" r:id="rId26" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{E807BF04-A66A-40A9-A97C-FAD54E6E5561}"/>
+    <hyperlink ref="A26" r:id="rId27" location="/case/CTDC-45349" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45349" xr:uid="{563C1C13-7FDB-48C6-A4F4-BAFD63F3620F}"/>
+    <hyperlink ref="B26" r:id="rId28" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{D7BA8C7E-F146-4E17-B12E-E859B9F0D4EE}"/>
+    <hyperlink ref="A13" r:id="rId29" location="/case/CTDC-45441" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45441" xr:uid="{03B8C3F3-6C0A-4A00-929D-15AE0F50B327}"/>
+    <hyperlink ref="B13" r:id="rId30" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{602CEABF-1995-4E17-AFBB-CFF7844E8264}"/>
+    <hyperlink ref="A42" r:id="rId31" location="/case/CTDC-45536" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45536" xr:uid="{5642849A-0897-47A8-A2BE-5EE1D176C1C3}"/>
+    <hyperlink ref="B42" r:id="rId32" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{DF770DAA-2339-47BF-9867-20967CA43B21}"/>
+    <hyperlink ref="A29" r:id="rId33" location="/case/CTDC-45544" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45544" xr:uid="{E256EDFA-003B-4197-A505-605A8821A225}"/>
+    <hyperlink ref="B29" r:id="rId34" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{82302861-7FC9-4914-92B6-55D43AD81FBE}"/>
+    <hyperlink ref="A14" r:id="rId35" location="/case/CTDC-45557" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45557" xr:uid="{81424373-8DDD-4E52-AE12-CD6349850946}"/>
+    <hyperlink ref="B14" r:id="rId36" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{E339C159-3C7E-4108-906A-9984C2664AE5}"/>
+    <hyperlink ref="A68" r:id="rId37" location="/case/CTDC-45569" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45569" xr:uid="{E4548520-3EE4-4CD5-9DA0-85092C6C2016}"/>
+    <hyperlink ref="B68" r:id="rId38" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{A66A3F8A-FD8D-4044-8839-4835FBECB59C}"/>
+    <hyperlink ref="A24" r:id="rId39" location="/case/CTDC-45633" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45633" xr:uid="{78AFDB87-AF77-447E-9985-2B23D795AD25}"/>
+    <hyperlink ref="B24" r:id="rId40" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{7922E70E-0278-42D5-8A85-060EDFDB50FF}"/>
+    <hyperlink ref="A32" r:id="rId41" location="/case/CTDC-45660" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45660" xr:uid="{B6561F7D-7D3D-42D6-A1E5-FFDEA070ABF9}"/>
+    <hyperlink ref="B32" r:id="rId42" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{E341FDF7-AE5A-468B-A2BD-9F37924ACD65}"/>
+    <hyperlink ref="A69" r:id="rId43" location="/case/CTDC-45677" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45677" xr:uid="{816769A7-393B-4A7B-9B58-D7412342CDCF}"/>
+    <hyperlink ref="B69" r:id="rId44" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{1854C16A-9B57-4D58-BE0F-4C9E8F3BA66B}"/>
+    <hyperlink ref="A54" r:id="rId45" location="/case/CTDC-45704" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45704" xr:uid="{F064DBE2-3B98-4779-AB72-35E25502B0FA}"/>
+    <hyperlink ref="B54" r:id="rId46" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{4CF838C3-3B51-4DBB-9AA6-DBC7C2238861}"/>
+    <hyperlink ref="A58" r:id="rId47" location="/case/CTDC-45713" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45713" xr:uid="{8E814128-1E33-4365-A28F-49C12CAC9D70}"/>
+    <hyperlink ref="B58" r:id="rId48" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{4E458CA8-8A80-44CD-9704-2D66926B45DE}"/>
+    <hyperlink ref="A15" r:id="rId49" location="/case/CTDC-45829" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45829" xr:uid="{B3C252AF-2AFF-4FB9-809B-E70C5B714722}"/>
+    <hyperlink ref="B15" r:id="rId50" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{B1420248-B861-4416-868F-07987053AE36}"/>
+    <hyperlink ref="A33" r:id="rId51" location="/case/CTDC-45974" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45974" xr:uid="{0C7E2462-242A-4838-B446-F489F047F01B}"/>
+    <hyperlink ref="B33" r:id="rId52" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{8D5749A6-D805-4336-B2C4-B231949CF323}"/>
+    <hyperlink ref="A11" r:id="rId53" location="/case/CTDC-45987" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-45987" xr:uid="{5D0454E7-E8FD-47CD-8E65-237FBC0E3524}"/>
+    <hyperlink ref="B11" r:id="rId54" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{EA5EDCB7-1747-4722-828C-95EA04B5FB8E}"/>
+    <hyperlink ref="A43" r:id="rId55" location="/case/CTDC-46029" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46029" xr:uid="{D3A41EFB-5410-4317-85C1-80C211154148}"/>
+    <hyperlink ref="B43" r:id="rId56" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{F6065261-BDF0-45F1-AEA6-CEE922D78895}"/>
+    <hyperlink ref="A5" r:id="rId57" location="/case/CTDC-46057" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46057" xr:uid="{6F9FB442-26E7-425F-80C8-A2C9722E67B4}"/>
+    <hyperlink ref="B5" r:id="rId58" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{D5BB1A52-9FA4-4F85-A4B6-6AA3165E9620}"/>
+    <hyperlink ref="A16" r:id="rId59" location="/case/CTDC-46063" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46063" xr:uid="{77A4E9C1-DCC6-4D96-A1EF-461F8FFC18F6}"/>
+    <hyperlink ref="B16" r:id="rId60" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{837580F5-7448-4325-AEE3-3492F0D8001D}"/>
+    <hyperlink ref="A6" r:id="rId61" location="/case/CTDC-46116" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46116" xr:uid="{187B9160-4A12-4425-A15B-C0D3BF555B10}"/>
+    <hyperlink ref="B6" r:id="rId62" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{F1C64830-7528-4531-B9F2-AE35BE223D13}"/>
+    <hyperlink ref="A2" r:id="rId63" location="/case/CTDC-46143" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46143" xr:uid="{FB3E2821-C91C-495F-B647-51F93DACC3E1}"/>
+    <hyperlink ref="B2" r:id="rId64" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{77729363-3FCF-4ABF-B7BA-DFCF7AA6AF2A}"/>
+    <hyperlink ref="A34" r:id="rId65" location="/case/CTDC-46172" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46172" xr:uid="{7500A4E4-1474-4368-A211-E83864B5EEB5}"/>
+    <hyperlink ref="B34" r:id="rId66" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{F90B8873-05F2-41FB-A113-8A675A466817}"/>
+    <hyperlink ref="A44" r:id="rId67" location="/case/CTDC-46296" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46296" xr:uid="{1ABE7BE0-5ADA-4A2D-90DC-37DFC210787F}"/>
+    <hyperlink ref="B44" r:id="rId68" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{BA8672CE-E5F2-4259-9BC0-B6416568BAF9}"/>
+    <hyperlink ref="A70" r:id="rId69" location="/case/CTDC-46310" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46310" xr:uid="{C25438A1-5858-45D2-AD51-A4E05D8DA7E7}"/>
+    <hyperlink ref="B70" r:id="rId70" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{FB2C7B6E-D6E3-4BEB-BF08-401C0E7EB22B}"/>
+    <hyperlink ref="A60" r:id="rId71" location="/case/CTDC-46340" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46340" xr:uid="{1C73F3B4-2593-4F6F-9EC9-07486D193D93}"/>
+    <hyperlink ref="B60" r:id="rId72" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{48C9DFE7-B8C3-4FD7-B028-50E1501979D5}"/>
+    <hyperlink ref="A3" r:id="rId73" location="/case/CTDC-46433" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46433" xr:uid="{65EA85B5-328B-4E05-99EE-D64189C1CA6D}"/>
+    <hyperlink ref="B3" r:id="rId74" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{50B49430-0F7E-414D-A71C-F546380B9C44}"/>
+    <hyperlink ref="A30" r:id="rId75" location="/case/CTDC-46456" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46456" xr:uid="{E6DBF439-8566-4AC1-9D78-E9C024B712D1}"/>
+    <hyperlink ref="B30" r:id="rId76" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{1CFC8010-5D3B-424A-86AE-20D0BDBEEBF1}"/>
+    <hyperlink ref="A55" r:id="rId77" location="/case/CTDC-46489" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46489" xr:uid="{F228C4E6-3E71-4EDE-B2C9-56E61C19DD6F}"/>
+    <hyperlink ref="B55" r:id="rId78" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{60664251-3155-4C67-9497-2EE74D6AED35}"/>
+    <hyperlink ref="A45" r:id="rId79" location="/case/CTDC-46500" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46500" xr:uid="{B2F150D8-C831-40EB-A9B5-078B6AC7ACAD}"/>
+    <hyperlink ref="B45" r:id="rId80" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{9F0B3A4F-F46A-4293-8BF9-9921CB1EBF7B}"/>
+    <hyperlink ref="A61" r:id="rId81" location="/case/CTDC-46654" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46654" xr:uid="{13CE6B3A-FA84-4C81-A4DC-E7425ABDF37C}"/>
+    <hyperlink ref="B61" r:id="rId82" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{4EC93CE5-F6D3-4256-A1CB-C9A5D73E74A0}"/>
+    <hyperlink ref="A62" r:id="rId83" location="/case/CTDC-46681" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46681" xr:uid="{B1E0E4D5-C6CA-4048-B06E-517BF3C26D58}"/>
+    <hyperlink ref="B62" r:id="rId84" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{718CE1DD-A772-45C3-91B8-665233272BC0}"/>
+    <hyperlink ref="A71" r:id="rId85" location="/case/CTDC-46730" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46730" xr:uid="{6F4CFE53-0935-41C3-B9D1-86037CC56BF7}"/>
+    <hyperlink ref="B71" r:id="rId86" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{C589BE4F-5AFD-49EF-B0A1-3CEDF72BDB14}"/>
+    <hyperlink ref="A46" r:id="rId87" location="/case/CTDC-46749" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46749" xr:uid="{FFA34921-902D-4D6A-8503-0A18134B30C1}"/>
+    <hyperlink ref="B46" r:id="rId88" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{C1B2427D-8085-48F0-8735-3AE94E06D300}"/>
+    <hyperlink ref="A47" r:id="rId89" location="/case/CTDC-46779" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46779" xr:uid="{DEEE6722-2D88-4955-8D32-13081C0351FC}"/>
+    <hyperlink ref="B47" r:id="rId90" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{029D0142-42D9-43EB-85BC-7EF9239FD9FE}"/>
+    <hyperlink ref="A35" r:id="rId91" location="/case/CTDC-46828" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46828" xr:uid="{B704FDD0-C18C-426B-B778-E2C269884470}"/>
+    <hyperlink ref="B35" r:id="rId92" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{03073D9C-1542-4842-83E1-832EF29C1C17}"/>
+    <hyperlink ref="A17" r:id="rId93" location="/case/CTDC-46968" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-46968" xr:uid="{24CEEA79-8DDC-425F-893D-2D3F6197DA8C}"/>
+    <hyperlink ref="B17" r:id="rId94" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{6929738B-B4AB-41DA-B897-52DEDB6C3C81}"/>
+    <hyperlink ref="A31" r:id="rId95" location="/case/CTDC-47398" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-47398" xr:uid="{B5796DF7-BDDA-48D0-8C95-C9EB0D118B4A}"/>
+    <hyperlink ref="B31" r:id="rId96" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{566DBE78-9527-4110-9B79-ED0063D3B188}"/>
+    <hyperlink ref="A48" r:id="rId97" location="/case/CTDC-47810" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-47810" xr:uid="{0BBC9A59-34CA-49B8-8C73-AA9DF7CFBCB7}"/>
+    <hyperlink ref="B48" r:id="rId98" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{EACF7A36-952A-4A6D-B5FC-E9C8D0A80917}"/>
+    <hyperlink ref="A36" r:id="rId99" location="/case/CTDC-47986" display="https://trialcommons-qa.cancer.gov/ - /case/CTDC-47986" xr:uid="{4F4D3262-3B6B-4033-BB7F-47B5B939EE00}"/>
+    <hyperlink ref="B36" r:id="rId100" location="/trial/NCT02465060" display="https://trialcommons-qa.cancer.gov/ - /trial/NCT02465060" xr:uid="{DCF5B4EF-55D3-4CEA-8DFD-2997B982E74D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>